<commit_message>
added emoticon to output
</commit_message>
<xml_diff>
--- a/bugsEnhancementTracking.xlsx
+++ b/bugsEnhancementTracking.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>#</t>
   </si>
@@ -86,6 +86,21 @@
   </si>
   <si>
     <t>fixed to "verse summarizer"</t>
+  </si>
+  <si>
+    <t>using ul instead</t>
+  </si>
+  <si>
+    <t>pill is smaller, text still big</t>
+  </si>
+  <si>
+    <t>add emoticon to mail tone</t>
+  </si>
+  <si>
+    <t>button close is not working</t>
+  </si>
+  <si>
+    <t>code is too slow to load - change from cdn to local resource</t>
   </si>
 </sst>
 </file>
@@ -404,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,6 +461,9 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -458,7 +476,13 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="1">
+        <v>37712</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -533,6 +557,21 @@
       </c>
       <c r="F7" s="1">
         <v>37712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>